<commit_message>
Created session key and store in the database
</commit_message>
<xml_diff>
--- a/Authentication.xlsx
+++ b/Authentication.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rebeckaforsberg/Desktop/Thesis/ClientServerCommunication/ClientServerCommunication/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\alexk\Thesis\ClientServerCommunication\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1820B2F0-E495-8142-A381-BEB13FCA4D25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A15965F-6FC6-464A-B245-94D80B6B8E5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="2244" yWindow="1104" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Authentication" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Username</t>
   </si>
@@ -31,31 +31,23 @@
     <t>Salt</t>
   </si>
   <si>
-    <t>kolonia</t>
-  </si>
-  <si>
-    <t>6008132132f2c9ab580e83b0c72382fc360506cd942b5b3f26d062a52595f1c48f874ec0da9dc16973fbe1a5e8cbb99c647a2ed9d1f69eb52a9e63eb75931435</t>
-  </si>
-  <si>
-    <t>RwkiUU0Wc7YkXJmVmZUi4A==</t>
-  </si>
-  <si>
-    <t>alex</t>
-  </si>
-  <si>
-    <t>a47f9d066fdff10cd40aea4fa5179fdcd6114ead63ea0d3732b6106f676468529aaf75b3042518f66a4ddc0f32eb4a9585bd7c03afb7659d1f846e92b5f2cadb</t>
-  </si>
-  <si>
-    <t>cl9PchN99+tap3w1NXruDg==</t>
+    <t>SessionKey</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color indexed="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color indexed="8"/>
       <name val="Calibri"/>
@@ -83,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -103,7 +96,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -399,48 +392,30 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="A1:C2"/>
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
-      </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>